<commit_message>
adding more data to chi-cycle-chart and order of using herbal teas for an organized diet
</commit_message>
<xml_diff>
--- a/szerv_meridianok.xlsx
+++ b/szerv_meridianok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ciklusok_osszesitett_sablon" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">Lep</t>
   </si>
   <si>
-    <t xml:space="preserve">Emésztés-felszívas-kiválasztás</t>
+    <t xml:space="preserve">emésztés-felszívas-kiválasztás</t>
   </si>
   <si>
     <t xml:space="preserve">vérraktár</t>
@@ -304,6 +304,48 @@
     <t xml:space="preserve">Szivburok</t>
   </si>
   <si>
+    <t xml:space="preserve">a koszorúérrel kapcsolatban álló keringési működések szabályozása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tápanyag-beviteli funkciók szabályozása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">séta, levegőzés, lélegzet-gyakorlatok</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">az oxigén-ellátás megnövelése, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">energiapályáink lelassulnak, felkészülünk az éjszakai pihenőre, érzékeink kifinomulnak</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">barátságos természet, humorosság, szociális érzékenység, újítókedv, ihlet, teljes agyi kapacitás kihasználása, méltányosság, döntési erő, bőkezűség, támasznyújtás, szándék és cselekedet összhangja, pártatlanság, bizalomteljesség, cselekedeti tisztaság, ösztönök uralása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fizikai erőfeszítés és sport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pszichés megbetegedések, szemproblémák, keringési zavarok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mellkasi szorító fájdalom, nyugtalanság, izomgörcsök, könyökfájdalom, kéz- és lábgörcsök, végtagzsibbadás, elmezavar, idegesség</t>
+  </si>
+  <si>
     <t xml:space="preserve">21:00 - 23:00</t>
   </si>
   <si>
@@ -404,7 +446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -442,6 +484,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -485,16 +533,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -503,11 +547,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -518,6 +562,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -539,23 +591,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -635,545 +687,728 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL24"/>
+  <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="29.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="41.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="39.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="41.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="42.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="27.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="44.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="29.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="41.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="39.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="41.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="42.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="41.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="63.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="4" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="6"/>
-      <c r="BK1" s="6"/>
-      <c r="BL1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+      <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="n">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11" t="s">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L12" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H15" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="n">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H18" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="10" t="s">
+      <c r="I18" s="12"/>
+      <c r="J18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K18" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11" t="s">
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="9"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B25" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C25" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="n">
+      <c r="D25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="18"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="18"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="18"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="11"/>
+      <c r="B32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="87">
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
@@ -1182,43 +1417,85 @@
     <mergeCell ref="F6:F9"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
     <mergeCell ref="J6:J9"/>
     <mergeCell ref="K6:K9"/>
     <mergeCell ref="L6:L9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="H25:H31"/>
+    <mergeCell ref="I25:I31"/>
+    <mergeCell ref="J25:J31"/>
+    <mergeCell ref="K25:K31"/>
+    <mergeCell ref="L25:L31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1237,7 +1514,7 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
@@ -1245,214 +1522,214 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="3.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="40.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="28.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="40.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="25.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="16" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="40.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="28.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="40.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="25.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="4" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="5" customFormat="true" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>81</v>
+      <c r="B1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>85</v>
+      <c r="B2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>89</v>
+      <c r="B3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="B4" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1460,8 +1737,8 @@
       <c r="A19" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2" t="s">
-        <v>105</v>
+      <c r="B27" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>